<commit_message>
Ajuste frame grafica y nueva tabla yd vs yr
</commit_message>
<xml_diff>
--- a/src/data/out/BASERADIAL/EJEMPLO_1.xlsx
+++ b/src/data/out/BASERADIAL/EJEMPLO_1.xlsx
@@ -507,7 +507,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -529,42 +529,26 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1.360097246462209</v>
+        <v>1.153293757320417</v>
       </c>
       <c r="B2" t="n">
-        <v>1.846301310123029</v>
+        <v>1.909013966963473</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1.780292094838397</v>
+        <v>1.823104031894046</v>
       </c>
       <c r="B3" t="n">
-        <v>1.52966256256462</v>
+        <v>1.772578201014941</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1.321816806030021</v>
+        <v>1.323049601760364</v>
       </c>
       <c r="B4" t="n">
-        <v>1.966593384009409</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>1.120274157603511</v>
-      </c>
-      <c r="B5" t="n">
-        <v>1.804121751388855</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>1.032302012171877</v>
-      </c>
-      <c r="B6" t="n">
-        <v>1.043088211822678</v>
+        <v>1.745282590241487</v>
       </c>
     </row>
   </sheetData>
@@ -616,7 +600,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
     </row>

</xml_diff>